<commit_message>
finishing the clean of the logs for the 3 parts :scrapping, ocr, and pipeline ; cleaning the whole project ; finished changing the path to dynamic path; finished managing the incrmental of the 3 parts : scrapping; ocr and pipeline ; testing the new way to scrape URL --> it is possible to do it automaiccaly.dynamically from a city
</commit_message>
<xml_diff>
--- a/Config/trip_config_test.xlsx
+++ b/Config/trip_config_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/focus_profond/GIT_repo/flight_price_tracker/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890987D6-19F7-D044-8C85-4B21129A9A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E39BF3E-FD6C-3141-8009-AF042328768D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20480" activeTab="1" xr2:uid="{19124265-0F5A-314C-B656-9442AACA6FAB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="167">
   <si>
     <t>trip</t>
   </si>
@@ -516,6 +516,27 @@
   </si>
   <si>
     <t>city_desti</t>
+  </si>
+  <si>
+    <t>BRU_CDG</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>CDG</t>
+  </si>
+  <si>
+    <t>https://www.google.com/travel/flights?hl=en&amp;q=Flights%20to%20{CDG}%20from%20{EZE}%20on%20%20oneway&amp;curr=EUR</t>
+  </si>
+  <si>
+    <t>https://www.google.com/travel/flights?hl=en&amp;q=Flights%20to%20{BRU}%20from%20{CDG}%20on%20%20oneway&amp;curr=EUR</t>
+  </si>
+  <si>
+    <t>https://www.google.com/travel/flights?hl=en&amp;q=Flights%20to%20{CDG}%20from%20{BRU}%20on%20%20oneway&amp;curr=EUR</t>
   </si>
 </sst>
 </file>
@@ -1639,10 +1660,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D26FF8-C4D9-B54E-9588-5A51E95943B3}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1770,7 +1791,6 @@
       <c r="G5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1962,9 +1982,7 @@
       <c r="G13" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>91</v>
-      </c>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -2413,7 +2431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -2436,7 +2454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -2459,7 +2477,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -2482,7 +2500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -2505,7 +2523,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2528,7 +2546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -2551,7 +2569,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2574,7 +2592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -2597,7 +2615,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -2620,7 +2638,49 @@
         <v>9</v>
       </c>
     </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" t="s">
+        <v>128</v>
+      </c>
+      <c r="E42" t="s">
+        <v>162</v>
+      </c>
+      <c r="F42" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" t="s">
+        <v>163</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I43" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I44" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H42" r:id="rId1" xr:uid="{11DE6D4F-7BDF-9A4C-9C60-48C1645A35E6}"/>
+    <hyperlink ref="I43" r:id="rId2" xr:uid="{D1183059-1667-024F-A3F2-0659AD220A65}"/>
+    <hyperlink ref="I44" r:id="rId3" xr:uid="{BDCED845-0066-A447-B8F6-AB7388F4A792}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>